<commit_message>
Made some minor changes into the side menu collapsed, side menu
</commit_message>
<xml_diff>
--- a/yt_multi_language_ui_validator/src/main/resources/data/verifyingSideMenuCollapsedLangAsInSettings.xlsx
+++ b/yt_multi_language_ui_validator/src/main/resources/data/verifyingSideMenuCollapsedLangAsInSettings.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sagar\youtube-multi-language-ui-validator-automation\yt_multi_language_ui_validator\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE912096-DDE8-44B0-9EA3-7BC44BB66F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C4D351-08C1-4829-AFA8-700B783E5E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2544" yWindow="1980" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Results" sheetId="1" r:id="rId1"/>
+    <sheet name="verifyingSideMenuCollapsedLangA" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Removing the extra spaces in the content of the side menu collapsed expected data sheet
</commit_message>
<xml_diff>
--- a/yt_multi_language_ui_validator/src/main/resources/data/verifyingSideMenuCollapsedLangAsInSettings.xlsx
+++ b/yt_multi_language_ui_validator/src/main/resources/data/verifyingSideMenuCollapsedLangAsInSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sagar\youtube-multi-language-ui-validator-automation\yt_multi_language_ui_validator\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C4D351-08C1-4829-AFA8-700B783E5E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16875E92-D4D3-425C-8D63-F7B873ACA924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2544" yWindow="1980" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="verifyingSideMenuCollapsedLangA" sheetId="1" r:id="rId1"/>
@@ -25,57 +25,30 @@
     <t>Afrikaans</t>
   </si>
   <si>
-    <t xml:space="preserve">Tuis Kortvideo's Intekeninge Myne </t>
-  </si>
-  <si>
     <t>Azərbaycan</t>
   </si>
   <si>
-    <t xml:space="preserve">Ev Shorts Abunəliklər Siz </t>
-  </si>
-  <si>
     <t>Bahasa Indonesia</t>
   </si>
   <si>
-    <t xml:space="preserve">Beranda Shorts Subscription Anda </t>
-  </si>
-  <si>
     <t>Bosanski</t>
   </si>
   <si>
-    <t xml:space="preserve">Početna stranica Shorts Pretplate Vi </t>
-  </si>
-  <si>
     <t>Català</t>
   </si>
   <si>
-    <t xml:space="preserve">Inici YouTube Shorts Subscripcions Tu </t>
-  </si>
-  <si>
     <t>Dansk</t>
   </si>
   <si>
-    <t xml:space="preserve">Start Shorts Abonnementer Dig </t>
-  </si>
-  <si>
     <t>Deutsch</t>
   </si>
   <si>
-    <t xml:space="preserve">Startseite Shorts Abos Mein YouTube </t>
-  </si>
-  <si>
     <t>Eesti</t>
   </si>
   <si>
-    <t xml:space="preserve">Avaleht Shorts Tellimused Teie </t>
-  </si>
-  <si>
     <t>English (India)</t>
   </si>
   <si>
-    <t xml:space="preserve">Home Shorts Subscriptions You </t>
-  </si>
-  <si>
     <t>English (UK)</t>
   </si>
   <si>
@@ -85,247 +58,274 @@
     <t>Español (España)</t>
   </si>
   <si>
-    <t xml:space="preserve">Inicio Shorts Suscripciones Tú </t>
-  </si>
-  <si>
     <t>Español (Latinoamérica)</t>
   </si>
   <si>
-    <t xml:space="preserve">Principal Shorts Suscripciones Tú </t>
-  </si>
-  <si>
     <t>Español (US)</t>
   </si>
   <si>
     <t>Euskara</t>
   </si>
   <si>
-    <t xml:space="preserve">Orri nagusia Shorts Harpidetzak Zu </t>
-  </si>
-  <si>
     <t>Français</t>
   </si>
   <si>
-    <t xml:space="preserve">Accueil Shorts Abonnements Vous </t>
-  </si>
-  <si>
     <t>Français (Canada)</t>
   </si>
   <si>
     <t>Hrvatski</t>
   </si>
   <si>
-    <t xml:space="preserve">Početna Shorts Pretplate Moje </t>
-  </si>
-  <si>
     <t>Íslenska</t>
   </si>
   <si>
-    <t xml:space="preserve">Heim Shorts Áskriftir Þú </t>
-  </si>
-  <si>
     <t>Italiano</t>
   </si>
   <si>
-    <t xml:space="preserve">Home Shorts Iscrizioni Tu </t>
-  </si>
-  <si>
     <t>Latviešu valoda</t>
   </si>
   <si>
-    <t xml:space="preserve">Sākums Shorts Abonementi Jūs </t>
-  </si>
-  <si>
     <t>Lietuvių</t>
   </si>
   <si>
-    <t xml:space="preserve">Pagrindinis Shorts Prenumeratos Jūs </t>
-  </si>
-  <si>
     <t>Magyar</t>
   </si>
   <si>
-    <t xml:space="preserve">Kezdőlap Shorts Feliratkozások Te </t>
-  </si>
-  <si>
     <t>Nederlands</t>
   </si>
   <si>
-    <t xml:space="preserve">Home Shorts Abonnementen Jij </t>
-  </si>
-  <si>
     <t>Polski</t>
   </si>
   <si>
-    <t xml:space="preserve">Główna Shorts Subskrypcje Ty </t>
-  </si>
-  <si>
     <t>Português</t>
   </si>
   <si>
-    <t xml:space="preserve">Início Shorts Subscrições Eu </t>
-  </si>
-  <si>
     <t>Português (Brasil)</t>
   </si>
   <si>
-    <t xml:space="preserve">Início Shorts Inscrições Você </t>
-  </si>
-  <si>
     <t>Shqip</t>
   </si>
   <si>
-    <t xml:space="preserve">Faqja e parë Shorts Abonimet Ti </t>
-  </si>
-  <si>
     <t>Slovenščina</t>
   </si>
   <si>
-    <t xml:space="preserve">Domača stran Kratki videoposnetki Naročnine Vi </t>
-  </si>
-  <si>
     <t>Suomi</t>
   </si>
   <si>
-    <t xml:space="preserve">Koti Shorts Tilaukset Sinä </t>
-  </si>
-  <si>
     <t>Svenska</t>
   </si>
   <si>
-    <t xml:space="preserve">Hem Shorts Prenumerationer Ditt YouTube </t>
-  </si>
-  <si>
     <t>Tiếng Việt</t>
   </si>
   <si>
-    <t xml:space="preserve">Trang chủ Shorts Kênh đăng ký Bạn </t>
-  </si>
-  <si>
     <t>Türkçe</t>
   </si>
   <si>
-    <t xml:space="preserve">Ana Sayfa Shorts Abonelikler Siz </t>
-  </si>
-  <si>
     <t>Беларуская</t>
   </si>
   <si>
-    <t xml:space="preserve">Галоўная старонка Shorts Падпіскі Вы </t>
-  </si>
-  <si>
     <t>Български</t>
   </si>
   <si>
-    <t xml:space="preserve">Начало Shorts Абонаменти Вие </t>
-  </si>
-  <si>
     <t>Русский</t>
   </si>
   <si>
-    <t xml:space="preserve">Главная Shorts Подписки Вы </t>
-  </si>
-  <si>
     <t>Українська</t>
   </si>
   <si>
-    <t xml:space="preserve">Головна YouTube Shorts Підписки Ви </t>
-  </si>
-  <si>
     <t>Ελληνικά</t>
   </si>
   <si>
-    <t xml:space="preserve">Αρχική Shorts Εγγραφές Εσείς </t>
-  </si>
-  <si>
     <t>Հայերեն</t>
   </si>
   <si>
-    <t xml:space="preserve">Սկիզբ Shorts Հետևում եմ Դուք </t>
-  </si>
-  <si>
     <t>עברית</t>
   </si>
   <si>
-    <t xml:space="preserve">דף הבית Shorts מינויים הדף שלי </t>
-  </si>
-  <si>
     <t>العربية</t>
   </si>
   <si>
-    <t xml:space="preserve">الصفحة الرئيسية Shorts الاشتراكات أنت </t>
-  </si>
-  <si>
     <t>فارسی</t>
   </si>
   <si>
-    <t xml:space="preserve">صفحه اصلی کوته‌ویدیوهای YouTube اشتراک‌ها شما </t>
-  </si>
-  <si>
     <t>हिन्दी</t>
   </si>
   <si>
-    <t xml:space="preserve">होम पेज Shorts सदस्यता आप </t>
-  </si>
-  <si>
     <t>বাংলা</t>
   </si>
   <si>
-    <t xml:space="preserve">হোম Shorts সাবস্ক্রিপশন আপনি </t>
-  </si>
-  <si>
     <t>ਪੰਜਾਬੀ</t>
   </si>
   <si>
-    <t xml:space="preserve">ਹੋਮ Shorts ਸਬਸਕ੍ਰਿਪਸ਼ਨਾਂ ਤੁਸੀਂ </t>
-  </si>
-  <si>
     <t>ગુજરાતી</t>
   </si>
   <si>
-    <t xml:space="preserve">હોમ Shorts સબ્સ્ક્રિપ્શન તમે </t>
-  </si>
-  <si>
     <t>தமிழ்</t>
   </si>
   <si>
-    <t xml:space="preserve">முகப்பு Shorts சந்தாக்கள் நீங்கள் </t>
-  </si>
-  <si>
     <t>తెలుగు</t>
   </si>
   <si>
-    <t xml:space="preserve">మొదటి ట్యాబ్ Shorts సబ్‌స్క్రిప్షన్‌లు ఖాతా </t>
-  </si>
-  <si>
     <t>中文 (简体)</t>
   </si>
   <si>
-    <t xml:space="preserve">首页 Shorts 订阅 我 </t>
-  </si>
-  <si>
     <t>中文 (繁體)</t>
   </si>
   <si>
-    <t xml:space="preserve">首頁 Shorts 訂閱內容 個人中心 </t>
-  </si>
-  <si>
     <t>中文 (香港)</t>
   </si>
   <si>
-    <t xml:space="preserve">主頁 Shorts 訂閱項目 個人中心 </t>
-  </si>
-  <si>
     <t>日本語</t>
   </si>
   <si>
-    <t xml:space="preserve">ホーム ショート 登録チャンネル マイページ </t>
-  </si>
-  <si>
     <t>한국어</t>
   </si>
   <si>
-    <t xml:space="preserve">홈 Shorts 구독 내 페이지 </t>
+    <t>Tuis Kortvideo's Intekeninge Myne</t>
+  </si>
+  <si>
+    <t>Ev Shorts Abunəliklər Siz</t>
+  </si>
+  <si>
+    <t>Beranda Shorts Subscription Anda</t>
+  </si>
+  <si>
+    <t>Početna stranica Shorts Pretplate Vi</t>
+  </si>
+  <si>
+    <t>Inici YouTube Shorts Subscripcions Tu</t>
+  </si>
+  <si>
+    <t>Start Shorts Abonnementer Dig</t>
+  </si>
+  <si>
+    <t>Startseite Shorts Abos Mein YouTube</t>
+  </si>
+  <si>
+    <t>Avaleht Shorts Tellimused Teie</t>
+  </si>
+  <si>
+    <t>Home Shorts Subscriptions You</t>
+  </si>
+  <si>
+    <t>Inicio Shorts Suscripciones Tú</t>
+  </si>
+  <si>
+    <t>Principal Shorts Suscripciones Tú</t>
+  </si>
+  <si>
+    <t>Orri nagusia Shorts Harpidetzak Zu</t>
+  </si>
+  <si>
+    <t>Accueil Shorts Abonnements Vous</t>
+  </si>
+  <si>
+    <t>Početna Shorts Pretplate Moje</t>
+  </si>
+  <si>
+    <t>Heim Shorts Áskriftir Þú</t>
+  </si>
+  <si>
+    <t>Home Shorts Iscrizioni Tu</t>
+  </si>
+  <si>
+    <t>Sākums Shorts Abonementi Jūs</t>
+  </si>
+  <si>
+    <t>Pagrindinis Shorts Prenumeratos Jūs</t>
+  </si>
+  <si>
+    <t>Kezdőlap Shorts Feliratkozások Te</t>
+  </si>
+  <si>
+    <t>Home Shorts Abonnementen Jij</t>
+  </si>
+  <si>
+    <t>Główna Shorts Subskrypcje Ty</t>
+  </si>
+  <si>
+    <t>Início Shorts Subscrições Eu</t>
+  </si>
+  <si>
+    <t>Início Shorts Inscrições Você</t>
+  </si>
+  <si>
+    <t>Faqja e parë Shorts Abonimet Ti</t>
+  </si>
+  <si>
+    <t>Domača stran Kratki videoposnetki Naročnine Vi</t>
+  </si>
+  <si>
+    <t>Koti Shorts Tilaukset Sinä</t>
+  </si>
+  <si>
+    <t>Hem Shorts Prenumerationer Ditt YouTube</t>
+  </si>
+  <si>
+    <t>Trang chủ Shorts Kênh đăng ký Bạn</t>
+  </si>
+  <si>
+    <t>Ana Sayfa Shorts Abonelikler Siz</t>
+  </si>
+  <si>
+    <t>Галоўная старонка Shorts Падпіскі Вы</t>
+  </si>
+  <si>
+    <t>Начало Shorts Абонаменти Вие</t>
+  </si>
+  <si>
+    <t>Главная Shorts Подписки Вы</t>
+  </si>
+  <si>
+    <t>Головна YouTube Shorts Підписки Ви</t>
+  </si>
+  <si>
+    <t>Αρχική Shorts Εγγραφές Εσείς</t>
+  </si>
+  <si>
+    <t>Սկիզբ Shorts Հետևում եմ Դուք</t>
+  </si>
+  <si>
+    <t>דף הבית Shorts מינויים הדף שלי</t>
+  </si>
+  <si>
+    <t>الصفحة الرئيسية Shorts الاشتراكات أنت</t>
+  </si>
+  <si>
+    <t>صفحه اصلی کوته‌ویدیوهای YouTube اشتراک‌ها شما</t>
+  </si>
+  <si>
+    <t>होम पेज Shorts सदस्यता आप</t>
+  </si>
+  <si>
+    <t>হোম Shorts সাবস্ক্রিপশন আপনি</t>
+  </si>
+  <si>
+    <t>ਹੋਮ Shorts ਸਬਸਕ੍ਰਿਪਸ਼ਨਾਂ ਤੁਸੀਂ</t>
+  </si>
+  <si>
+    <t>હોમ Shorts સબ્સ્ક્રિપ્શન તમે</t>
+  </si>
+  <si>
+    <t>முகப்பு Shorts சந்தாக்கள் நீங்கள்</t>
+  </si>
+  <si>
+    <t>మొదటి ట్యాబ్ Shorts సబ్‌స్క్రిప్షన్‌లు ఖాతా</t>
+  </si>
+  <si>
+    <t>首页 Shorts 订阅 我</t>
+  </si>
+  <si>
+    <t>首頁 Shorts 訂閱內容 個人中心</t>
+  </si>
+  <si>
+    <t>主頁 Shorts 訂閱項目 個人中心</t>
+  </si>
+  <si>
+    <t>ホーム ショート 登録チャンネル マイページ</t>
+  </si>
+  <si>
+    <t>홈 Shorts 구독 내 페이지</t>
   </si>
 </sst>
 </file>
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,420 +694,420 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="B54" t="s">
         <v>101</v>

</xml_diff>